<commit_message>
baseline module column name updates
for use in new mass flows
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/LiteratureInstallationProjections.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/LiteratureInstallationProjections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE5EA0E-6E35-44DC-8242-77FE958DC938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A769BC-A3B0-43D6-95F7-11F5B7A66DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5DE1FCD1-9D64-4446-91DA-0961A3088D24}"/>
+    <workbookView xWindow="30960" yWindow="2160" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{5DE1FCD1-9D64-4446-91DA-0961A3088D24}"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -147,6 +147,9 @@
   <si>
     <t>newInstalledCapacity_SF-LvR_48years &amp; 70% Recycled_[MW]</t>
   </si>
+  <si>
+    <t>https://irena.org/Statistics/View-Data-by-Topic/Energy-Transition/REmap-Energy-Generation-and-Capacity</t>
+  </si>
 </sst>
 </file>
 
@@ -243,7 +246,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -255,6 +258,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -264,7 +268,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="%" xfId="2" xr:uid="{81452E6B-F638-4287-8B73-D95A6C474FC8}"/>
@@ -4605,7 +4611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BB4D31-3979-4EF5-B9D0-3C27811932A1}">
   <dimension ref="A1:Y84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L4" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -4621,7 +4627,7 @@
     <col min="9" max="9" width="12.6328125" customWidth="1"/>
     <col min="10" max="10" width="11.08984375" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="10"/>
+    <col min="12" max="12" width="8.7265625" style="7"/>
     <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.81640625" style="4" customWidth="1"/>
     <col min="15" max="15" width="11.08984375" bestFit="1" customWidth="1"/>
@@ -4636,42 +4642,42 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="10" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="8" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -4690,7 +4696,7 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="7">
         <v>1200.6513499999901</v>
       </c>
       <c r="M2" t="s">
@@ -4746,7 +4752,7 @@
       <c r="K3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="7">
         <v>2534.3001088300002</v>
       </c>
       <c r="M3" t="s">
@@ -4816,7 +4822,7 @@
         <f>I4*1000</f>
         <v>131000</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="7">
         <v>2534.3001088300002</v>
       </c>
       <c r="M4" s="4">
@@ -4897,7 +4903,7 @@
         <f t="shared" ref="K5:K34" si="2">I5*1000</f>
         <v>154000</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="7">
         <v>5123.0323208</v>
       </c>
       <c r="M5" s="4">
@@ -4981,7 +4987,7 @@
         <f t="shared" si="2"/>
         <v>177000</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="7">
         <v>5123.0323208</v>
       </c>
       <c r="M6" s="4">
@@ -5065,7 +5071,7 @@
         <f t="shared" si="2"/>
         <v>200000</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>9477.5425046749897</v>
       </c>
       <c r="M7" s="4">
@@ -5149,7 +5155,7 @@
         <f t="shared" si="2"/>
         <v>223000</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="7">
         <v>9477.5425046749897</v>
       </c>
       <c r="M8" s="4">
@@ -5236,7 +5242,7 @@
         <f t="shared" si="2"/>
         <v>249000</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="7">
         <v>9156.77890338</v>
       </c>
       <c r="M9" s="4">
@@ -5320,7 +5326,7 @@
         <f t="shared" si="2"/>
         <v>275000</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="7">
         <v>9156.77890338</v>
       </c>
       <c r="M10" s="4">
@@ -5404,7 +5410,7 @@
         <f t="shared" si="2"/>
         <v>301000</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="7">
         <v>16995.842998244902</v>
       </c>
       <c r="M11" s="4">
@@ -5488,7 +5494,7 @@
         <f t="shared" si="2"/>
         <v>327000</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>16995.842998244902</v>
       </c>
       <c r="M12" s="4">
@@ -5572,7 +5578,7 @@
         <f t="shared" si="2"/>
         <v>353000</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="7">
         <v>4723.5930226999899</v>
       </c>
       <c r="M13" s="4">
@@ -5659,7 +5665,7 @@
         <f t="shared" si="2"/>
         <v>383000</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="7">
         <v>4723.5930226999899</v>
       </c>
       <c r="M14" s="4">
@@ -5743,7 +5749,7 @@
         <f t="shared" si="2"/>
         <v>413000</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="7">
         <v>34173.144328415001</v>
       </c>
       <c r="M15" s="4">
@@ -5827,7 +5833,7 @@
         <f t="shared" si="2"/>
         <v>443000</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="7">
         <v>34173.144328415001</v>
       </c>
       <c r="M16" s="4">
@@ -5911,7 +5917,7 @@
         <f t="shared" si="2"/>
         <v>473000</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="7">
         <v>73232.04575818</v>
       </c>
       <c r="M17" s="4">
@@ -5995,7 +6001,7 @@
         <f t="shared" si="2"/>
         <v>503000</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="7">
         <v>73232.04575818</v>
       </c>
       <c r="M18" s="4">
@@ -6082,7 +6088,7 @@
         <f t="shared" si="2"/>
         <v>528000</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="7">
         <v>61963.949007384901</v>
       </c>
       <c r="M19" s="4">
@@ -6166,7 +6172,7 @@
         <f t="shared" si="2"/>
         <v>553000</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="7">
         <v>61963.949007384901</v>
       </c>
       <c r="M20" s="4">
@@ -6250,7 +6256,7 @@
         <f t="shared" si="2"/>
         <v>578000</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="7">
         <v>81314.849570864899</v>
       </c>
       <c r="M21" s="4">
@@ -6334,7 +6340,7 @@
         <f t="shared" si="2"/>
         <v>603000</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="7">
         <v>81314.849570864899</v>
       </c>
       <c r="M22" s="4">
@@ -6405,7 +6411,7 @@
         <f t="shared" si="2"/>
         <v>628000</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="7">
         <v>49200.342204749897</v>
       </c>
       <c r="M23" s="4">
@@ -6479,7 +6485,7 @@
         <f t="shared" si="2"/>
         <v>661000</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="7">
         <v>49200.342204749897</v>
       </c>
       <c r="M24" s="4">
@@ -6550,7 +6556,7 @@
         <f t="shared" si="2"/>
         <v>694000</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="7">
         <v>100734.892095405</v>
       </c>
       <c r="M25" s="4">
@@ -6621,7 +6627,7 @@
         <f t="shared" si="2"/>
         <v>727000</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="7">
         <v>100734.892095405</v>
       </c>
       <c r="M26" s="4">
@@ -6692,7 +6698,7 @@
         <f t="shared" si="2"/>
         <v>760000</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27" s="7">
         <v>89886.844265459993</v>
       </c>
       <c r="M27" s="4">
@@ -6763,7 +6769,7 @@
         <f t="shared" si="2"/>
         <v>793000</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="7">
         <v>89886.844265459993</v>
       </c>
       <c r="M28" s="4">
@@ -6837,7 +6843,7 @@
         <f t="shared" si="2"/>
         <v>843000</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="7">
         <v>59996.065785355</v>
       </c>
       <c r="M29" s="4">
@@ -6908,7 +6914,7 @@
         <f t="shared" si="2"/>
         <v>893000</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="7">
         <v>59996.065785355</v>
       </c>
       <c r="M30" s="4">
@@ -6979,7 +6985,7 @@
         <f t="shared" si="2"/>
         <v>943000</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="7">
         <v>13613.503684884899</v>
       </c>
       <c r="M31" s="4">
@@ -7050,7 +7056,7 @@
         <f t="shared" si="2"/>
         <v>993000</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="7">
         <v>13613.503684884899</v>
       </c>
       <c r="M32" s="4">
@@ -7121,7 +7127,7 @@
         <f t="shared" si="2"/>
         <v>1043000</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33" s="7">
         <v>36887.263406979997</v>
       </c>
       <c r="M33" s="4">
@@ -7195,7 +7201,7 @@
         <f t="shared" si="2"/>
         <v>1093000</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="7">
         <v>36887.263406979997</v>
       </c>
       <c r="M34" s="4">
@@ -7239,7 +7245,7 @@
         <v>1671.5511811464301</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="L35" s="10">
+      <c r="L35" s="7">
         <v>44331.142776660003</v>
       </c>
       <c r="N35" s="4">
@@ -7256,7 +7262,7 @@
         <v>1392.9593176220251</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="L36" s="10">
+      <c r="L36" s="7">
         <v>44331.142776660003</v>
       </c>
     </row>
@@ -7265,7 +7271,7 @@
         <v>2053</v>
       </c>
       <c r="D37" s="4"/>
-      <c r="L37" s="10">
+      <c r="L37" s="7">
         <v>71991.796050289995</v>
       </c>
     </row>
@@ -7273,7 +7279,7 @@
       <c r="A38">
         <v>2054</v>
       </c>
-      <c r="L38" s="10">
+      <c r="L38" s="7">
         <v>71991.796050289995</v>
       </c>
     </row>
@@ -7281,7 +7287,7 @@
       <c r="A39">
         <v>2055</v>
       </c>
-      <c r="L39" s="10">
+      <c r="L39" s="7">
         <v>42648.336863960001</v>
       </c>
     </row>
@@ -7289,7 +7295,7 @@
       <c r="A40">
         <v>2056</v>
       </c>
-      <c r="L40" s="10">
+      <c r="L40" s="7">
         <v>42648.336863960001</v>
       </c>
     </row>
@@ -7297,7 +7303,7 @@
       <c r="A41">
         <v>2057</v>
       </c>
-      <c r="L41" s="10">
+      <c r="L41" s="7">
         <v>69993.457237224895</v>
       </c>
     </row>
@@ -7305,7 +7311,7 @@
       <c r="A42">
         <v>2058</v>
       </c>
-      <c r="L42" s="10">
+      <c r="L42" s="7">
         <v>69993.457237224895</v>
       </c>
     </row>
@@ -7537,8 +7543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B749E6-E878-4161-8BD8-61B2A1558660}">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7546,34 +7553,39 @@
     <col min="1" max="1" width="8.7265625" style="4"/>
     <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="10"/>
       <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="F2"/>
       <c r="H2" s="4" t="s">

</xml_diff>

<commit_message>
updates to working on cell tech compare
not a lot of progress, reorg
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/LiteratureInstallationProjections.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/LiteratureInstallationProjections.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A769BC-A3B0-43D6-95F7-11F5B7A66DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC4DA98-A4C1-4C13-B271-DB878DE798CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30960" yWindow="2160" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{5DE1FCD1-9D64-4446-91DA-0961A3088D24}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5DE1FCD1-9D64-4446-91DA-0961A3088D24}"/>
   </bookViews>
   <sheets>
     <sheet name="US" sheetId="1" r:id="rId1"/>
@@ -260,6 +260,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyAlignment="1">
@@ -267,9 +270,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4642,42 +4642,42 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="9" t="s">
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -7545,7 +7545,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="C8"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7565,25 +7565,25 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="11"/>
       <c r="H1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="5"/>

</xml_diff>

<commit_message>
Completed global projection thru 2100
with linear increase to approx 60 TW in 2100, and IRENA historical numbers, and 50 TW in 2050
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/LiteratureInstallationProjections.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/LiteratureInstallationProjections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D74F20-CAAD-43F3-BDB3-EBF634516BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C8FDED-0125-441E-8183-7DDEFA2391D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{5DE1FCD1-9D64-4446-91DA-0961A3088D24}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>year</t>
   </si>
@@ -166,6 +166,27 @@
   <si>
     <t>PWhr/yr</t>
   </si>
+  <si>
+    <t>https://ember-climate.org/data/data-explorer/</t>
+  </si>
+  <si>
+    <t>World Installed Capacity by source, total absolute GW</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Cumulative</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>Linear Projected Increase</t>
+  </si>
+  <si>
+    <t>MW cumulative</t>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +197,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +236,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
@@ -269,7 +299,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -285,9 +315,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -302,6 +329,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="%" xfId="2" xr:uid="{81452E6B-F638-4287-8B73-D95A6C474FC8}"/>
@@ -3810,6 +3841,326 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="80"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10353002024237344"/>
+                  <c:y val="-7.9822249941529588E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2050to2100Estimates'!$M$2:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2050to2100Estimates'!$N$2:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3123.5871032069999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7729.2653366454897</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C59-4E4F-AEB0-1E940F1F3075}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="515381152"/>
+        <c:axId val="515381480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="515381152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515381480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="515381480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515381152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3970,6 +4321,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5519,6 +5910,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6158,7 +7065,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -6180,6 +7087,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>31749</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9208236B-D889-0796-CF60-50A84FD69CF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6517,42 +7460,42 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="L1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="12" t="s">
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" t="s">
@@ -9435,18 +10378,18 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="14"/>
       <c r="H1" t="s">
         <v>28</v>
       </c>
@@ -10515,18 +11458,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137580ED-C83E-47BE-992D-E9B23297BB0E}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="13" max="13" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.90625" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -10539,8 +11483,19 @@
       <c r="H1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="J1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="8">
         <v>2000.0848697413501</v>
       </c>
@@ -10553,15 +11508,27 @@
       <c r="H2" s="8">
         <v>82.162162162162105</v>
       </c>
-      <c r="L2">
+      <c r="J2" s="15">
         <v>2050</v>
       </c>
-      <c r="M2">
+      <c r="K2" s="15">
         <f>50*1000000</f>
         <v>50000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="L2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2">
+        <v>2000</v>
+      </c>
+      <c r="N2">
+        <v>3123.5871032069999</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="8">
         <v>2019.73455933379</v>
       </c>
@@ -10580,15 +11547,30 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="L3">
+      <c r="J3" s="15">
         <v>2100</v>
       </c>
-      <c r="M3" s="9">
-        <f>1.532*(L3-L2)+M2</f>
-        <v>50000076.600000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="K3" s="16">
+        <f>219.32*1000*(J3-J2)+K2</f>
+        <v>60966000</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3">
+        <v>2021</v>
+      </c>
+      <c r="N3">
+        <v>7729.2653366454897</v>
+      </c>
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="8">
         <v>2049.3986439597102</v>
       </c>
@@ -10602,7 +11584,7 @@
         <v>158.82063882063801</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="G5" s="8">
         <v>2023.5886302680101</v>
       </c>
@@ -10610,8 +11592,8 @@
         <v>124.226044226044</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="N7" s="10"/>
+    <row r="7" spans="1:16">
+      <c r="L7" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>